<commit_message>
Actualización CN 07 01
Actualización CN 07 01
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/Escaleta_CN_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/Escaleta_CN_07_01_CO.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Dropbox\Editorial planeta\1. Autor\Escaletas\CN_07_01_CO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
-    <sheet name="DATOS" sheetId="1" r:id="rId2"/>
+    <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$2:$U$42</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -471,12 +477,6 @@
     <t>Actividad que permite identificar las características del movimiento en los procariotas</t>
   </si>
   <si>
-    <t>El movimiento en los organismos procariotas</t>
-  </si>
-  <si>
-    <t>Actividad de preguntas que permite repasar las características del movimiento en arqueas y bacterias</t>
-  </si>
-  <si>
     <t>Recurso M4A-01</t>
   </si>
   <si>
@@ -528,9 +528,6 @@
     <t>Las estructuras de la locomoción en protozoos</t>
   </si>
   <si>
-    <t>Actividad del juego del ahorcado que permite repasar las estructuras de locomoción en protozoos</t>
-  </si>
-  <si>
     <t>Recurso M14A-01</t>
   </si>
   <si>
@@ -543,9 +540,6 @@
     <t>El movimiento en las algas</t>
   </si>
   <si>
-    <t>Actividad de completar un texto relacionado con el movimiento en las algas</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: La locomoción en protistas</t>
   </si>
   <si>
@@ -588,9 +582,6 @@
     <t>Los tipos de tropismos</t>
   </si>
   <si>
-    <t>Interactivo que permite identificar los tropismos que presentan las plantas antes los estímulos externos</t>
-  </si>
-  <si>
     <t>Actividad de relacionar frases que describen los tropismos en las plantas</t>
   </si>
   <si>
@@ -672,9 +663,6 @@
     <t>Clasifica los animales según su esqueleto</t>
   </si>
   <si>
-    <t>Actividad que permite clasificar algunos animales según el esqueleto que posea</t>
-  </si>
-  <si>
     <t>Recurso M10B-01</t>
   </si>
   <si>
@@ -807,20 +795,38 @@
     <t>Actividad que propone diferenciar las estrategias del movimiento en animales</t>
   </si>
   <si>
-    <t>Competencias: comprensión del movimiento en microorganismos</t>
-  </si>
-  <si>
-    <t>Actividad que propone reconocer las estructuras que permiten el movimiento en microorganismos</t>
-  </si>
-  <si>
     <t>Actividad que propone un experimento para observar y comprender el movimiento en las plantas</t>
+  </si>
+  <si>
+    <t>El movimiento en bacterias y arqueas</t>
+  </si>
+  <si>
+    <t>Actividad de preguntas que permite repasar las características del movimiento en bacterias y arqueas</t>
+  </si>
+  <si>
+    <t>Actividad del juego del ahorcado que permite reconocer las estructuras de locomoción en protozoos</t>
+  </si>
+  <si>
+    <t>Actividad para completar un texto relacionado con el movimiento en las algas</t>
+  </si>
+  <si>
+    <t>Interactivo que permite identificar los tropismos que presentan las plantas ante los estímulos externos</t>
+  </si>
+  <si>
+    <t>Actividad que permite clasificar algunos animales según el esqueleto que posean</t>
+  </si>
+  <si>
+    <t>Competencias: formulación de preguntas en el método científico</t>
+  </si>
+  <si>
+    <t>Actividad que permite comprender la etapa de formulación de preguntas en un experimento utilizando el método científico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -855,6 +861,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -976,7 +998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1039,34 +1061,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1106,6 +1116,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1168,7 +1196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1201,9 +1229,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1236,6 +1281,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1414,9 +1476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,95 +1505,95 @@
     <col min="21" max="21" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:21" s="16" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="48"/>
-      <c r="O1" s="28" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="P1" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="Q1" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="S1" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="T1" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="U1" s="47" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="16" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="43"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="17" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="31"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1628,7 +1690,7 @@
         <v>8</v>
       </c>
       <c r="M4" s="8"/>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="29" t="s">
         <v>121</v>
       </c>
       <c r="O4" s="9"/>
@@ -1759,7 +1821,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="8"/>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="29" t="s">
         <v>23</v>
       </c>
       <c r="O7" s="9"/>
@@ -1820,7 +1882,7 @@
         <v>8</v>
       </c>
       <c r="M8" s="8"/>
-      <c r="N8" s="8" t="s">
+      <c r="N8" s="29" t="s">
         <v>27</v>
       </c>
       <c r="O8" s="9"/>
@@ -1863,7 +1925,7 @@
         <v>144</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>150</v>
+        <v>257</v>
       </c>
       <c r="H9" s="19">
         <v>5</v>
@@ -1872,7 +1934,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>151</v>
+        <v>258</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>20</v>
@@ -1898,7 +1960,7 @@
         <v>135</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="U9" s="10" t="s">
         <v>137</v>
@@ -1922,7 +1984,7 @@
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H10" s="19">
         <v>6</v>
@@ -1931,7 +1993,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1957,7 +2019,7 @@
         <v>135</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="U10" s="10" t="s">
         <v>137</v>
@@ -1974,13 +2036,13 @@
         <v>122</v>
       </c>
       <c r="D11" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" s="22" t="s">
         <v>156</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>158</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="19"/>
@@ -2009,13 +2071,13 @@
         <v>122</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E12" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>157</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>159</v>
       </c>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
@@ -2044,16 +2106,16 @@
         <v>122</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H13" s="19">
         <v>7</v>
@@ -2062,7 +2124,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>19</v>
@@ -2070,12 +2132,12 @@
       <c r="L13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="28" t="s">
         <v>62</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="P13" s="19" t="s">
         <v>19</v>
@@ -2084,16 +2146,16 @@
         <v>7</v>
       </c>
       <c r="R13" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S13" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="T13" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="S13" s="25" t="s">
+      <c r="U13" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="T13" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="U13" s="10" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2107,16 +2169,16 @@
         <v>122</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H14" s="19">
         <v>8</v>
@@ -2125,7 +2187,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>169</v>
+        <v>259</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2151,7 +2213,7 @@
         <v>135</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="U14" s="10" t="s">
         <v>137</v>
@@ -2168,14 +2230,14 @@
         <v>122</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="21" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H15" s="19">
         <v>9</v>
@@ -2184,7 +2246,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>174</v>
+        <v>260</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2210,7 +2272,7 @@
         <v>135</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="U15" s="10" t="s">
         <v>137</v>
@@ -2227,14 +2289,14 @@
         <v>122</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>132</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H16" s="19">
         <v>10</v>
@@ -2243,7 +2305,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2253,7 +2315,7 @@
       </c>
       <c r="M16" s="8"/>
       <c r="N16" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="19" t="s">
@@ -2269,7 +2331,7 @@
         <v>135</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="U16" s="10" t="s">
         <v>137</v>
@@ -2286,10 +2348,10 @@
         <v>122</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="21"/>
@@ -2319,16 +2381,16 @@
         <v>122</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H18" s="19">
         <v>11</v>
@@ -2337,7 +2399,7 @@
         <v>19</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>189</v>
+        <v>261</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2357,16 +2419,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2380,16 +2442,16 @@
         <v>122</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="H19" s="19">
         <v>12</v>
@@ -2398,7 +2460,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2424,7 +2486,7 @@
         <v>135</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="U19" s="10" t="s">
         <v>137</v>
@@ -2441,25 +2503,25 @@
         <v>122</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H20" s="19">
         <v>13</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2468,7 +2530,7 @@
         <v>5</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="N20" s="8"/>
       <c r="O20" s="9"/>
@@ -2479,16 +2541,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -2502,16 +2564,16 @@
         <v>122</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H21" s="19">
         <v>14</v>
@@ -2520,7 +2582,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2546,7 +2608,7 @@
         <v>135</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="U21" s="10" t="s">
         <v>137</v>
@@ -2563,16 +2625,16 @@
         <v>122</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F22" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="G22" s="21" t="s">
         <v>198</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>203</v>
       </c>
       <c r="H22" s="19">
         <v>15</v>
@@ -2581,7 +2643,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2607,7 +2669,7 @@
         <v>135</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="U22" s="10" t="s">
         <v>137</v>
@@ -2624,14 +2686,14 @@
         <v>122</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>132</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="21" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H23" s="19">
         <v>16</v>
@@ -2640,7 +2702,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2650,7 +2712,7 @@
       </c>
       <c r="M23" s="8"/>
       <c r="N23" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="19" t="s">
@@ -2666,7 +2728,7 @@
         <v>135</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="U23" s="10" t="s">
         <v>137</v>
@@ -2683,13 +2745,13 @@
         <v>122</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="19"/>
@@ -2718,13 +2780,13 @@
         <v>122</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G25" s="21"/>
       <c r="H25" s="19"/>
@@ -2753,16 +2815,16 @@
         <v>122</v>
       </c>
       <c r="D26" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="G26" s="21" t="s">
         <v>208</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>213</v>
       </c>
       <c r="H26" s="19">
         <v>17</v>
@@ -2771,7 +2833,7 @@
         <v>19</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
@@ -2791,16 +2853,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="T26" s="12" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2814,16 +2876,16 @@
         <v>122</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H27" s="19">
         <v>18</v>
@@ -2832,7 +2894,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>217</v>
+        <v>262</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
@@ -2858,7 +2920,7 @@
         <v>135</v>
       </c>
       <c r="T27" s="12" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U27" s="10" t="s">
         <v>137</v>
@@ -2875,14 +2937,14 @@
         <v>122</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="F28" s="22"/>
       <c r="G28" s="21" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="H28" s="19">
         <v>19</v>
@@ -2891,7 +2953,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -2917,7 +2979,7 @@
         <v>135</v>
       </c>
       <c r="T28" s="12" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="U28" s="10" t="s">
         <v>137</v>
@@ -2934,13 +2996,13 @@
         <v>122</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="19"/>
@@ -2969,13 +3031,13 @@
         <v>122</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G30" s="21"/>
       <c r="H30" s="19"/>
@@ -3004,13 +3066,13 @@
         <v>122</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="G31" s="21"/>
       <c r="H31" s="19"/>
@@ -3039,16 +3101,16 @@
         <v>122</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H32" s="19">
         <v>20</v>
@@ -3057,7 +3119,7 @@
         <v>19</v>
       </c>
       <c r="J32" s="18" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>19</v>
@@ -3065,7 +3127,7 @@
       <c r="L32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M32" s="8" t="s">
+      <c r="M32" s="28" t="s">
         <v>62</v>
       </c>
       <c r="N32" s="8"/>
@@ -3077,16 +3139,16 @@
         <v>5</v>
       </c>
       <c r="R32" s="11" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="S32" s="10" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="T32" s="12" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3100,13 +3162,13 @@
         <v>122</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G33" s="21"/>
       <c r="H33" s="19"/>
@@ -3135,16 +3197,16 @@
         <v>122</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E34" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="F34" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="F34" s="22" t="s">
-        <v>229</v>
-      </c>
       <c r="G34" s="21" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H34" s="19">
         <v>21</v>
@@ -3153,7 +3215,7 @@
         <v>19</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3173,16 +3235,16 @@
         <v>6</v>
       </c>
       <c r="R34" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="S34" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="T34" s="12" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="U34" s="10" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3196,16 +3258,16 @@
         <v>122</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E35" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="F35" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="G35" s="21" t="s">
         <v>229</v>
-      </c>
-      <c r="G35" s="21" t="s">
-        <v>235</v>
       </c>
       <c r="H35" s="19">
         <v>22</v>
@@ -3214,7 +3276,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="18" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3240,7 +3302,7 @@
         <v>135</v>
       </c>
       <c r="T35" s="12" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="U35" s="10" t="s">
         <v>137</v>
@@ -3257,14 +3319,14 @@
         <v>122</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>132</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="21" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="H36" s="19">
         <v>23</v>
@@ -3273,7 +3335,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="K36" s="7" t="s">
         <v>20</v>
@@ -3283,7 +3345,7 @@
       </c>
       <c r="M36" s="8"/>
       <c r="N36" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="19" t="s">
@@ -3299,7 +3361,7 @@
         <v>135</v>
       </c>
       <c r="T36" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="U36" s="10" t="s">
         <v>137</v>
@@ -3316,12 +3378,12 @@
         <v>122</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="22"/>
       <c r="G37" s="21" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="H37" s="19">
         <v>24</v>
@@ -3330,7 +3392,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>20</v>
@@ -3340,7 +3402,7 @@
       </c>
       <c r="M37" s="8"/>
       <c r="N37" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="O37" s="9"/>
       <c r="P37" s="19" t="s">
@@ -3356,7 +3418,7 @@
         <v>135</v>
       </c>
       <c r="T37" s="12" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="U37" s="10" t="s">
         <v>137</v>
@@ -3373,12 +3435,12 @@
         <v>122</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E38" s="13"/>
       <c r="F38" s="22"/>
       <c r="G38" s="21" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="H38" s="19">
         <v>25</v>
@@ -3387,7 +3449,7 @@
         <v>20</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="K38" s="7" t="s">
         <v>20</v>
@@ -3397,7 +3459,7 @@
       </c>
       <c r="M38" s="8"/>
       <c r="N38" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="O38" s="9"/>
       <c r="P38" s="19" t="s">
@@ -3413,13 +3475,13 @@
         <v>135</v>
       </c>
       <c r="T38" s="12" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="U38" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>17</v>
       </c>
@@ -3430,12 +3492,12 @@
         <v>122</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E39" s="13"/>
       <c r="F39" s="22"/>
       <c r="G39" s="21" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="H39" s="19">
         <v>26</v>
@@ -3444,7 +3506,7 @@
         <v>20</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="K39" s="7" t="s">
         <v>20</v>
@@ -3454,7 +3516,7 @@
       </c>
       <c r="M39" s="8"/>
       <c r="N39" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="O39" s="9"/>
       <c r="P39" s="19" t="s">
@@ -3470,7 +3532,7 @@
         <v>135</v>
       </c>
       <c r="T39" s="12" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="U39" s="10" t="s">
         <v>137</v>
@@ -3487,12 +3549,12 @@
         <v>122</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E40" s="13"/>
       <c r="F40" s="22"/>
       <c r="G40" s="21" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="H40" s="19">
         <v>27</v>
@@ -3501,7 +3563,7 @@
         <v>20</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="K40" s="7" t="s">
         <v>20</v>
@@ -3532,12 +3594,12 @@
         <v>122</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E41" s="13"/>
       <c r="F41" s="22"/>
       <c r="G41" s="21" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="H41" s="19">
         <v>28</v>
@@ -3546,7 +3608,7 @@
         <v>20</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="K41" s="7" t="s">
         <v>20</v>
@@ -3572,7 +3634,7 @@
         <v>135</v>
       </c>
       <c r="T41" s="12" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="U41" s="10" t="s">
         <v>137</v>
@@ -3589,12 +3651,12 @@
         <v>122</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E42" s="13"/>
       <c r="F42" s="22"/>
       <c r="G42" s="21" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H42" s="19">
         <v>29</v>
@@ -3603,7 +3665,7 @@
         <v>20</v>
       </c>
       <c r="J42" s="18" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="K42" s="7" t="s">
         <v>20</v>
@@ -3613,7 +3675,7 @@
       </c>
       <c r="M42" s="8"/>
       <c r="N42" s="8" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="O42" s="9"/>
       <c r="P42" s="24" t="s">
@@ -3629,7 +3691,7 @@
         <v>135</v>
       </c>
       <c r="T42" s="12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="U42" s="10" t="s">
         <v>137</v>
@@ -4641,10 +4703,14 @@
     <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:U42">
-    <filterColumn colId="12" showButton="0"/>
-  </autoFilter>
+  <autoFilter ref="A2:U42"/>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4659,12 +4725,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>